<commit_message>
fixes to distored hierarchy
Signed-off-by: Pawel Garbacz <pawel.garbacz@makolab.com>
</commit_message>
<xml_diff>
--- a/bdot10k_ontology/cellfie_import_data/bdot10k_import.xlsx
+++ b/bdot10k_ontology/cellfie_import_data/bdot10k_import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel.garbacz\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ihpan\urbanonto\bdot10k_ontology\cellfie_import_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0CFDA3-93AB-4141-AB27-7D37DEFC5336}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97969C5A-0CF1-4F1D-BEEA-8DB9E74BE5D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_import" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3707,48 +3706,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akcent 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akcent 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akcent 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akcent 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akcent 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akcent 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Dane wejściowe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Dane wyjściowe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Dobry" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Komórka połączona" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Komórka zaznaczona" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Nagłówek 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Nagłówek 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Nagłówek 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Nagłówek 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutralny" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Obliczenia" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Suma" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Tekst objaśnienia" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Tekst ostrzeżenia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Tytuł" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Uwaga" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Zły" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3764,9 +3763,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3804,7 +3803,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3910,7 +3909,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4176,7 +4175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDC7384-6DC3-481F-8CFA-2DA36A169F64}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -4993,8 +4992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3787C0-90B6-49C7-93CF-6A3BCCB384EB}">
   <dimension ref="A1:D286"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D279" sqref="D279"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106:B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6477,7 +6476,7 @@
         <v>595</v>
       </c>
       <c r="B106" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C106" t="s">
         <v>163</v>
@@ -6491,7 +6490,7 @@
         <v>596</v>
       </c>
       <c r="B107" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C107" t="s">
         <v>165</v>
@@ -6505,7 +6504,7 @@
         <v>597</v>
       </c>
       <c r="B108" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C108" t="s">
         <v>166</v>
@@ -6519,7 +6518,7 @@
         <v>598</v>
       </c>
       <c r="B109" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C109" t="s">
         <v>168</v>
@@ -6533,7 +6532,7 @@
         <v>599</v>
       </c>
       <c r="B110" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C110" t="s">
         <v>170</v>
@@ -6547,7 +6546,7 @@
         <v>600</v>
       </c>
       <c r="B111" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C111" t="s">
         <v>172</v>
@@ -6561,7 +6560,7 @@
         <v>601</v>
       </c>
       <c r="B112" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C112" t="s">
         <v>174</v>
@@ -6575,7 +6574,7 @@
         <v>602</v>
       </c>
       <c r="B113" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C113" t="s">
         <v>176</v>
@@ -6589,7 +6588,7 @@
         <v>603</v>
       </c>
       <c r="B114" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C114" t="s">
         <v>178</v>
@@ -6603,7 +6602,7 @@
         <v>604</v>
       </c>
       <c r="B115" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C115" t="s">
         <v>179</v>
@@ -6617,7 +6616,7 @@
         <v>605</v>
       </c>
       <c r="B116" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C116" t="s">
         <v>181</v>
@@ -6631,7 +6630,7 @@
         <v>606</v>
       </c>
       <c r="B117" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C117" t="s">
         <v>182</v>
@@ -6645,7 +6644,7 @@
         <v>607</v>
       </c>
       <c r="B118" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C118" t="s">
         <v>183</v>
@@ -6659,7 +6658,7 @@
         <v>608</v>
       </c>
       <c r="B119" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C119" t="s">
         <v>185</v>
@@ -6673,7 +6672,7 @@
         <v>609</v>
       </c>
       <c r="B120" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C120" t="s">
         <v>187</v>
@@ -6687,7 +6686,7 @@
         <v>610</v>
       </c>
       <c r="B121" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C121" t="s">
         <v>189</v>
@@ -6701,7 +6700,7 @@
         <v>611</v>
       </c>
       <c r="B122" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C122" t="s">
         <v>191</v>
@@ -6715,7 +6714,7 @@
         <v>612</v>
       </c>
       <c r="B123" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C123" t="s">
         <v>193</v>
@@ -6729,7 +6728,7 @@
         <v>613</v>
       </c>
       <c r="B124" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C124" t="s">
         <v>195</v>
@@ -6743,7 +6742,7 @@
         <v>614</v>
       </c>
       <c r="B125" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C125" t="s">
         <v>197</v>
@@ -6757,7 +6756,7 @@
         <v>615</v>
       </c>
       <c r="B126" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C126" t="s">
         <v>199</v>

</xml_diff>